<commit_message>
Ajustes excel 1.1 logo
</commit_message>
<xml_diff>
--- a/excel/ponto.xlsx
+++ b/excel/ponto.xlsx
@@ -8,7 +8,9 @@
   <sheets>
     <sheet name="capa" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="abertura" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Encerramento" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="795.412.3-1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="819.027.5-2" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Encerramento" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="125725" fullCalcOnLoad="1"/>
@@ -240,7 +242,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -374,6 +376,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,6 +393,66 @@
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>1</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="666750" cy="666750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>1</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="666750" cy="666750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -804,6 +876,2386 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:T48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="3" bestFit="1" customWidth="1" style="20" min="1" max="1"/>
+    <col width="5.42578125" bestFit="1" customWidth="1" style="20" min="2" max="2"/>
+    <col width="26.7109375" customWidth="1" style="20" min="3" max="3"/>
+    <col width="2.7109375" customWidth="1" style="20" min="4" max="18"/>
+    <col width="13.7109375" customWidth="1" style="20" min="19" max="19"/>
+    <col width="6.28515625" customWidth="1" style="20" min="20" max="20"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="16" t="n"/>
+      <c r="B1" s="17" t="n"/>
+      <c r="C1" s="17" t="n"/>
+      <c r="D1" s="17" t="n"/>
+      <c r="E1" s="17" t="n"/>
+      <c r="F1" s="17" t="n"/>
+      <c r="G1" s="17" t="n"/>
+      <c r="H1" s="17" t="n"/>
+      <c r="I1" s="17" t="n"/>
+      <c r="J1" s="17" t="n"/>
+      <c r="K1" s="17" t="n"/>
+      <c r="L1" s="17" t="n"/>
+      <c r="M1" s="17" t="n"/>
+      <c r="N1" s="17" t="n"/>
+      <c r="O1" s="17" t="n"/>
+      <c r="P1" s="17" t="n"/>
+      <c r="Q1" s="17" t="n"/>
+      <c r="R1" s="17" t="n"/>
+      <c r="S1" s="17" t="n"/>
+      <c r="T1" s="18" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="19" t="n"/>
+      <c r="T2" s="21" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="19" t="n"/>
+      <c r="T3" s="21" t="n"/>
+    </row>
+    <row r="4" ht="15.75" customHeight="1" s="20" thickBot="1">
+      <c r="A4" s="22" t="n"/>
+      <c r="B4" s="23" t="n"/>
+      <c r="C4" s="23" t="n"/>
+      <c r="D4" s="23" t="n"/>
+      <c r="E4" s="23" t="n"/>
+      <c r="F4" s="23" t="n"/>
+      <c r="G4" s="23" t="n"/>
+      <c r="H4" s="23" t="n"/>
+      <c r="I4" s="23" t="n"/>
+      <c r="J4" s="23" t="n"/>
+      <c r="K4" s="23" t="n"/>
+      <c r="L4" s="23" t="n"/>
+      <c r="M4" s="23" t="n"/>
+      <c r="N4" s="23" t="n"/>
+      <c r="O4" s="23" t="n"/>
+      <c r="P4" s="23" t="n"/>
+      <c r="Q4" s="23" t="n"/>
+      <c r="R4" s="23" t="n"/>
+      <c r="S4" s="23" t="inlineStr">
+        <is>
+          <t>Março 2020</t>
+        </is>
+      </c>
+      <c r="T4" s="24" t="n"/>
+    </row>
+    <row r="5" ht="8.1" customHeight="1" s="20" thickBot="1"/>
+    <row r="6" ht="30" customHeight="1" s="20">
+      <c r="A6" s="41" t="inlineStr">
+        <is>
+          <t>NOME</t>
+        </is>
+      </c>
+      <c r="B6" s="17" t="n"/>
+      <c r="C6" s="30" t="inlineStr">
+        <is>
+          <t>ELOIZA DA SILVA SOUZA</t>
+        </is>
+      </c>
+      <c r="D6" s="42" t="inlineStr">
+        <is>
+          <t>RF/Vinculo</t>
+        </is>
+      </c>
+      <c r="E6" s="17" t="n"/>
+      <c r="F6" s="17" t="n"/>
+      <c r="G6" s="17" t="n"/>
+      <c r="H6" s="47" t="inlineStr">
+        <is>
+          <t>795.412.3/1</t>
+        </is>
+      </c>
+      <c r="I6" s="17" t="n"/>
+      <c r="J6" s="17" t="n"/>
+      <c r="K6" s="17" t="n"/>
+      <c r="L6" s="38" t="inlineStr">
+        <is>
+          <t>Estrutura Hierárquica</t>
+        </is>
+      </c>
+      <c r="M6" s="17" t="n"/>
+      <c r="N6" s="17" t="n"/>
+      <c r="O6" s="17" t="n"/>
+      <c r="P6" s="17" t="n"/>
+      <c r="Q6" s="17" t="n"/>
+      <c r="R6" s="17" t="n"/>
+      <c r="S6" s="59" t="inlineStr">
+        <is>
+          <t>162500000630000</t>
+        </is>
+      </c>
+      <c r="T6" s="18" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CARGO </t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Professor Educ. Infantil e Ens. Fund. I</t>
+        </is>
+      </c>
+      <c r="D7" s="44" t="inlineStr">
+        <is>
+          <t>QPE</t>
+        </is>
+      </c>
+      <c r="H7" s="45" t="inlineStr">
+        <is>
+          <t>18B</t>
+        </is>
+      </c>
+      <c r="L7" s="44" t="inlineStr">
+        <is>
+          <t>JORNADA</t>
+        </is>
+      </c>
+      <c r="S7" s="46" t="inlineStr">
+        <is>
+          <t>JEIF</t>
+        </is>
+      </c>
+      <c r="T7" s="21" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="48" t="inlineStr">
+        <is>
+          <t>regência</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>11:00 - 15:00 HS</t>
+        </is>
+      </c>
+      <c r="D8" s="44" t="inlineStr">
+        <is>
+          <t>hor. Coletivo</t>
+        </is>
+      </c>
+      <c r="I8" s="45" t="inlineStr">
+        <is>
+          <t>12:30 - 14:00 HS</t>
+        </is>
+      </c>
+      <c r="S8" s="44" t="inlineStr">
+        <is>
+          <t>turma</t>
+        </is>
+      </c>
+      <c r="T8" s="46" t="inlineStr">
+        <is>
+          <t>5B/5F</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="15.75" customHeight="1" s="20" thickBot="1">
+      <c r="A9" s="50" t="inlineStr">
+        <is>
+          <t>H.A / H.I</t>
+        </is>
+      </c>
+      <c r="B9" s="23" t="n"/>
+      <c r="C9" s="53" t="inlineStr">
+        <is>
+          <t>segunda 10:15 - 11:00; quarta 10:15 - 11:00hs</t>
+        </is>
+      </c>
+      <c r="D9" s="23" t="n"/>
+      <c r="E9" s="23" t="n"/>
+      <c r="F9" s="23" t="n"/>
+      <c r="G9" s="23" t="n"/>
+      <c r="H9" s="23" t="n"/>
+      <c r="I9" s="23" t="n"/>
+      <c r="J9" s="23" t="n"/>
+      <c r="K9" s="23" t="n"/>
+      <c r="L9" s="23" t="n"/>
+      <c r="M9" s="23" t="n"/>
+      <c r="N9" s="23" t="n"/>
+      <c r="O9" s="23" t="n"/>
+      <c r="P9" s="23" t="n"/>
+      <c r="Q9" s="23" t="n"/>
+      <c r="R9" s="23" t="n"/>
+      <c r="S9" s="23" t="n"/>
+      <c r="T9" s="24" t="n"/>
+    </row>
+    <row r="10" ht="16.5" customHeight="1" s="20"/>
+    <row r="11">
+      <c r="A11" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" s="25" t="inlineStr">
+        <is>
+          <t>Dom</t>
+        </is>
+      </c>
+      <c r="C11" s="60" t="n"/>
+      <c r="D11" s="60" t="n"/>
+      <c r="E11" s="60" t="n"/>
+      <c r="F11" s="60" t="n"/>
+      <c r="G11" s="60" t="n"/>
+      <c r="H11" s="60" t="n"/>
+      <c r="I11" s="60" t="n"/>
+      <c r="J11" s="60" t="n"/>
+      <c r="K11" s="61" t="n"/>
+      <c r="L11" s="61" t="n"/>
+      <c r="M11" s="61" t="n"/>
+      <c r="N11" s="61" t="n"/>
+      <c r="O11" s="61" t="n"/>
+      <c r="P11" s="61" t="n"/>
+      <c r="Q11" s="61" t="n"/>
+      <c r="R11" s="61" t="n"/>
+      <c r="S11" s="62" t="n"/>
+      <c r="T11" s="61" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" s="25" t="inlineStr">
+        <is>
+          <t>Seg</t>
+        </is>
+      </c>
+      <c r="C12" s="25" t="n"/>
+      <c r="D12" s="25" t="n"/>
+      <c r="E12" s="25" t="n"/>
+      <c r="F12" s="25" t="n"/>
+      <c r="G12" s="25" t="n"/>
+      <c r="H12" s="25" t="n"/>
+      <c r="I12" s="25" t="n"/>
+      <c r="J12" s="25" t="n"/>
+      <c r="K12" s="27" t="n"/>
+      <c r="L12" s="27" t="n"/>
+      <c r="M12" s="27" t="n"/>
+      <c r="N12" s="27" t="n"/>
+      <c r="O12" s="27" t="n"/>
+      <c r="P12" s="27" t="n"/>
+      <c r="Q12" s="27" t="n"/>
+      <c r="R12" s="27" t="n"/>
+      <c r="S12" s="58" t="n"/>
+      <c r="T12" s="27" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="B13" s="25" t="inlineStr">
+        <is>
+          <t>Ter</t>
+        </is>
+      </c>
+      <c r="C13" s="25" t="n"/>
+      <c r="D13" s="25" t="n"/>
+      <c r="E13" s="25" t="n"/>
+      <c r="F13" s="25" t="n"/>
+      <c r="G13" s="25" t="n"/>
+      <c r="H13" s="26" t="n"/>
+      <c r="I13" s="25" t="n"/>
+      <c r="J13" s="25" t="n"/>
+      <c r="K13" s="27" t="n"/>
+      <c r="L13" s="27" t="n"/>
+      <c r="M13" s="27" t="n"/>
+      <c r="N13" s="27" t="n"/>
+      <c r="O13" s="27" t="n"/>
+      <c r="P13" s="27" t="n"/>
+      <c r="Q13" s="27" t="n"/>
+      <c r="R13" s="27" t="n"/>
+      <c r="S13" s="58" t="n"/>
+      <c r="T13" s="27" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="B14" s="25" t="inlineStr">
+        <is>
+          <t>Qua</t>
+        </is>
+      </c>
+      <c r="C14" s="25" t="n"/>
+      <c r="D14" s="25" t="n"/>
+      <c r="E14" s="25" t="n"/>
+      <c r="F14" s="25" t="n"/>
+      <c r="G14" s="25" t="n"/>
+      <c r="H14" s="25" t="n"/>
+      <c r="I14" s="25" t="n"/>
+      <c r="J14" s="25" t="n"/>
+      <c r="K14" s="27" t="n"/>
+      <c r="L14" s="27" t="n"/>
+      <c r="M14" s="27" t="n"/>
+      <c r="N14" s="27" t="n"/>
+      <c r="O14" s="27" t="n"/>
+      <c r="P14" s="27" t="n"/>
+      <c r="Q14" s="27" t="n"/>
+      <c r="R14" s="27" t="n"/>
+      <c r="S14" s="58" t="n"/>
+      <c r="T14" s="27" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="25" t="n">
+        <v>5</v>
+      </c>
+      <c r="B15" s="25" t="inlineStr">
+        <is>
+          <t>Qui</t>
+        </is>
+      </c>
+      <c r="C15" s="25" t="n"/>
+      <c r="D15" s="25" t="n"/>
+      <c r="E15" s="25" t="n"/>
+      <c r="F15" s="25" t="n"/>
+      <c r="G15" s="25" t="n"/>
+      <c r="H15" s="25" t="n"/>
+      <c r="I15" s="25" t="n"/>
+      <c r="J15" s="25" t="n"/>
+      <c r="K15" s="27" t="n"/>
+      <c r="L15" s="27" t="n"/>
+      <c r="M15" s="27" t="n"/>
+      <c r="N15" s="27" t="n"/>
+      <c r="O15" s="27" t="n"/>
+      <c r="P15" s="27" t="n"/>
+      <c r="Q15" s="27" t="n"/>
+      <c r="R15" s="27" t="n"/>
+      <c r="S15" s="58" t="n"/>
+      <c r="T15" s="27" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="25" t="n">
+        <v>6</v>
+      </c>
+      <c r="B16" s="25" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="C16" s="25" t="n"/>
+      <c r="D16" s="25" t="n"/>
+      <c r="E16" s="25" t="n"/>
+      <c r="F16" s="25" t="n"/>
+      <c r="G16" s="25" t="n"/>
+      <c r="H16" s="25" t="n"/>
+      <c r="I16" s="25" t="n"/>
+      <c r="J16" s="25" t="n"/>
+      <c r="K16" s="27" t="n"/>
+      <c r="L16" s="27" t="n"/>
+      <c r="M16" s="27" t="n"/>
+      <c r="N16" s="27" t="n"/>
+      <c r="O16" s="27" t="n"/>
+      <c r="P16" s="27" t="n"/>
+      <c r="Q16" s="27" t="n"/>
+      <c r="R16" s="27" t="n"/>
+      <c r="S16" s="58" t="n"/>
+      <c r="T16" s="27" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="B17" s="25" t="inlineStr">
+        <is>
+          <t>Sáb</t>
+        </is>
+      </c>
+      <c r="C17" s="60" t="n"/>
+      <c r="D17" s="60" t="n"/>
+      <c r="E17" s="60" t="n"/>
+      <c r="F17" s="60" t="n"/>
+      <c r="G17" s="60" t="n"/>
+      <c r="H17" s="60" t="n"/>
+      <c r="I17" s="60" t="n"/>
+      <c r="J17" s="60" t="n"/>
+      <c r="K17" s="61" t="n"/>
+      <c r="L17" s="61" t="n"/>
+      <c r="M17" s="61" t="n"/>
+      <c r="N17" s="61" t="n"/>
+      <c r="O17" s="61" t="n"/>
+      <c r="P17" s="61" t="n"/>
+      <c r="Q17" s="61" t="n"/>
+      <c r="R17" s="61" t="n"/>
+      <c r="S17" s="62" t="n"/>
+      <c r="T17" s="61" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="B18" s="25" t="inlineStr">
+        <is>
+          <t>Dom</t>
+        </is>
+      </c>
+      <c r="C18" s="60" t="n"/>
+      <c r="D18" s="60" t="n"/>
+      <c r="E18" s="60" t="n"/>
+      <c r="F18" s="60" t="n"/>
+      <c r="G18" s="60" t="n"/>
+      <c r="H18" s="60" t="n"/>
+      <c r="I18" s="60" t="n"/>
+      <c r="J18" s="60" t="n"/>
+      <c r="K18" s="61" t="n"/>
+      <c r="L18" s="61" t="n"/>
+      <c r="M18" s="61" t="n"/>
+      <c r="N18" s="61" t="n"/>
+      <c r="O18" s="61" t="n"/>
+      <c r="P18" s="61" t="n"/>
+      <c r="Q18" s="61" t="n"/>
+      <c r="R18" s="61" t="n"/>
+      <c r="S18" s="62" t="n"/>
+      <c r="T18" s="61" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="25" t="n">
+        <v>9</v>
+      </c>
+      <c r="B19" s="25" t="inlineStr">
+        <is>
+          <t>Seg</t>
+        </is>
+      </c>
+      <c r="C19" s="25" t="n"/>
+      <c r="D19" s="25" t="n"/>
+      <c r="E19" s="25" t="n"/>
+      <c r="F19" s="25" t="n"/>
+      <c r="G19" s="25" t="n"/>
+      <c r="H19" s="25" t="n"/>
+      <c r="I19" s="25" t="n"/>
+      <c r="J19" s="25" t="n"/>
+      <c r="K19" s="27" t="n"/>
+      <c r="L19" s="27" t="n"/>
+      <c r="M19" s="27" t="n"/>
+      <c r="N19" s="27" t="n"/>
+      <c r="O19" s="27" t="n"/>
+      <c r="P19" s="27" t="n"/>
+      <c r="Q19" s="27" t="n"/>
+      <c r="R19" s="27" t="n"/>
+      <c r="S19" s="58" t="n"/>
+      <c r="T19" s="27" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="25" t="n">
+        <v>10</v>
+      </c>
+      <c r="B20" s="25" t="inlineStr">
+        <is>
+          <t>Ter</t>
+        </is>
+      </c>
+      <c r="C20" s="25" t="n"/>
+      <c r="D20" s="25" t="n"/>
+      <c r="E20" s="25" t="n"/>
+      <c r="F20" s="25" t="n"/>
+      <c r="G20" s="25" t="n"/>
+      <c r="H20" s="25" t="n"/>
+      <c r="I20" s="25" t="n"/>
+      <c r="J20" s="25" t="n"/>
+      <c r="K20" s="27" t="n"/>
+      <c r="L20" s="27" t="n"/>
+      <c r="M20" s="27" t="n"/>
+      <c r="N20" s="27" t="n"/>
+      <c r="O20" s="27" t="n"/>
+      <c r="P20" s="27" t="n"/>
+      <c r="Q20" s="27" t="n"/>
+      <c r="R20" s="27" t="n"/>
+      <c r="S20" s="58" t="n"/>
+      <c r="T20" s="27" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="25" t="n">
+        <v>11</v>
+      </c>
+      <c r="B21" s="25" t="inlineStr">
+        <is>
+          <t>Qua</t>
+        </is>
+      </c>
+      <c r="C21" s="25" t="n"/>
+      <c r="D21" s="25" t="n"/>
+      <c r="E21" s="25" t="n"/>
+      <c r="F21" s="25" t="n"/>
+      <c r="G21" s="25" t="n"/>
+      <c r="H21" s="25" t="n"/>
+      <c r="I21" s="25" t="n"/>
+      <c r="J21" s="25" t="n"/>
+      <c r="K21" s="27" t="n"/>
+      <c r="L21" s="27" t="n"/>
+      <c r="M21" s="27" t="n"/>
+      <c r="N21" s="27" t="n"/>
+      <c r="O21" s="27" t="n"/>
+      <c r="P21" s="27" t="n"/>
+      <c r="Q21" s="27" t="n"/>
+      <c r="R21" s="27" t="n"/>
+      <c r="S21" s="58" t="n"/>
+      <c r="T21" s="27" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="25" t="n">
+        <v>12</v>
+      </c>
+      <c r="B22" s="25" t="inlineStr">
+        <is>
+          <t>Qui</t>
+        </is>
+      </c>
+      <c r="C22" s="25" t="n"/>
+      <c r="D22" s="25" t="n"/>
+      <c r="E22" s="25" t="n"/>
+      <c r="F22" s="25" t="n"/>
+      <c r="G22" s="25" t="n"/>
+      <c r="H22" s="25" t="n"/>
+      <c r="I22" s="25" t="n"/>
+      <c r="J22" s="25" t="n"/>
+      <c r="K22" s="27" t="n"/>
+      <c r="L22" s="27" t="n"/>
+      <c r="M22" s="27" t="n"/>
+      <c r="N22" s="27" t="n"/>
+      <c r="O22" s="27" t="n"/>
+      <c r="P22" s="27" t="n"/>
+      <c r="Q22" s="27" t="n"/>
+      <c r="R22" s="27" t="n"/>
+      <c r="S22" s="58" t="n"/>
+      <c r="T22" s="27" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="25" t="n">
+        <v>13</v>
+      </c>
+      <c r="B23" s="25" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="C23" s="25" t="n"/>
+      <c r="D23" s="25" t="n"/>
+      <c r="E23" s="25" t="n"/>
+      <c r="F23" s="25" t="n"/>
+      <c r="G23" s="25" t="n"/>
+      <c r="H23" s="25" t="n"/>
+      <c r="I23" s="25" t="n"/>
+      <c r="J23" s="25" t="n"/>
+      <c r="K23" s="27" t="n"/>
+      <c r="L23" s="27" t="n"/>
+      <c r="M23" s="27" t="n"/>
+      <c r="N23" s="27" t="n"/>
+      <c r="O23" s="27" t="n"/>
+      <c r="P23" s="27" t="n"/>
+      <c r="Q23" s="27" t="n"/>
+      <c r="R23" s="27" t="n"/>
+      <c r="S23" s="58" t="n"/>
+      <c r="T23" s="27" t="n"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="25" t="n">
+        <v>14</v>
+      </c>
+      <c r="B24" s="25" t="inlineStr">
+        <is>
+          <t>Sáb</t>
+        </is>
+      </c>
+      <c r="C24" s="60" t="n"/>
+      <c r="D24" s="60" t="n"/>
+      <c r="E24" s="60" t="n"/>
+      <c r="F24" s="60" t="n"/>
+      <c r="G24" s="60" t="n"/>
+      <c r="H24" s="60" t="n"/>
+      <c r="I24" s="60" t="n"/>
+      <c r="J24" s="60" t="n"/>
+      <c r="K24" s="61" t="n"/>
+      <c r="L24" s="61" t="n"/>
+      <c r="M24" s="61" t="n"/>
+      <c r="N24" s="61" t="n"/>
+      <c r="O24" s="61" t="n"/>
+      <c r="P24" s="61" t="n"/>
+      <c r="Q24" s="61" t="n"/>
+      <c r="R24" s="61" t="n"/>
+      <c r="S24" s="62" t="n"/>
+      <c r="T24" s="61" t="n"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="25" t="n">
+        <v>15</v>
+      </c>
+      <c r="B25" s="25" t="inlineStr">
+        <is>
+          <t>Dom</t>
+        </is>
+      </c>
+      <c r="C25" s="60" t="n"/>
+      <c r="D25" s="60" t="n"/>
+      <c r="E25" s="60" t="n"/>
+      <c r="F25" s="60" t="n"/>
+      <c r="G25" s="60" t="n"/>
+      <c r="H25" s="60" t="n"/>
+      <c r="I25" s="60" t="n"/>
+      <c r="J25" s="60" t="n"/>
+      <c r="K25" s="61" t="n"/>
+      <c r="L25" s="61" t="n"/>
+      <c r="M25" s="61" t="n"/>
+      <c r="N25" s="61" t="n"/>
+      <c r="O25" s="61" t="n"/>
+      <c r="P25" s="61" t="n"/>
+      <c r="Q25" s="61" t="n"/>
+      <c r="R25" s="61" t="n"/>
+      <c r="S25" s="62" t="n"/>
+      <c r="T25" s="61" t="n"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="25" t="n">
+        <v>16</v>
+      </c>
+      <c r="B26" s="25" t="inlineStr">
+        <is>
+          <t>Seg</t>
+        </is>
+      </c>
+      <c r="C26" s="25" t="n"/>
+      <c r="D26" s="25" t="n"/>
+      <c r="E26" s="25" t="n"/>
+      <c r="F26" s="25" t="n"/>
+      <c r="G26" s="25" t="n"/>
+      <c r="H26" s="25" t="n"/>
+      <c r="I26" s="25" t="n"/>
+      <c r="J26" s="25" t="n"/>
+      <c r="K26" s="27" t="n"/>
+      <c r="L26" s="27" t="n"/>
+      <c r="M26" s="27" t="n"/>
+      <c r="N26" s="27" t="n"/>
+      <c r="O26" s="27" t="n"/>
+      <c r="P26" s="27" t="n"/>
+      <c r="Q26" s="27" t="n"/>
+      <c r="R26" s="27" t="n"/>
+      <c r="S26" s="58" t="n"/>
+      <c r="T26" s="27" t="n"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="25" t="n">
+        <v>17</v>
+      </c>
+      <c r="B27" s="25" t="inlineStr">
+        <is>
+          <t>Ter</t>
+        </is>
+      </c>
+      <c r="C27" s="25" t="n"/>
+      <c r="D27" s="25" t="n"/>
+      <c r="E27" s="25" t="n"/>
+      <c r="F27" s="25" t="n"/>
+      <c r="G27" s="25" t="n"/>
+      <c r="H27" s="25" t="n"/>
+      <c r="I27" s="25" t="n"/>
+      <c r="J27" s="25" t="n"/>
+      <c r="K27" s="27" t="n"/>
+      <c r="L27" s="27" t="n"/>
+      <c r="M27" s="27" t="n"/>
+      <c r="N27" s="27" t="n"/>
+      <c r="O27" s="27" t="n"/>
+      <c r="P27" s="27" t="n"/>
+      <c r="Q27" s="27" t="n"/>
+      <c r="R27" s="27" t="n"/>
+      <c r="S27" s="58" t="n"/>
+      <c r="T27" s="27" t="n"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="25" t="n">
+        <v>18</v>
+      </c>
+      <c r="B28" s="25" t="inlineStr">
+        <is>
+          <t>Qua</t>
+        </is>
+      </c>
+      <c r="C28" s="25" t="n"/>
+      <c r="D28" s="25" t="n"/>
+      <c r="E28" s="25" t="n"/>
+      <c r="F28" s="25" t="n"/>
+      <c r="G28" s="25" t="n"/>
+      <c r="H28" s="25" t="n"/>
+      <c r="I28" s="25" t="n"/>
+      <c r="J28" s="25" t="n"/>
+      <c r="K28" s="27" t="n"/>
+      <c r="L28" s="27" t="n"/>
+      <c r="M28" s="27" t="n"/>
+      <c r="N28" s="27" t="n"/>
+      <c r="O28" s="27" t="n"/>
+      <c r="P28" s="27" t="n"/>
+      <c r="Q28" s="27" t="n"/>
+      <c r="R28" s="27" t="n"/>
+      <c r="S28" s="58" t="n"/>
+      <c r="T28" s="27" t="n"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="25" t="n">
+        <v>19</v>
+      </c>
+      <c r="B29" s="25" t="inlineStr">
+        <is>
+          <t>Qui</t>
+        </is>
+      </c>
+      <c r="C29" s="25" t="n"/>
+      <c r="D29" s="25" t="n"/>
+      <c r="E29" s="25" t="n"/>
+      <c r="F29" s="25" t="n"/>
+      <c r="G29" s="25" t="n"/>
+      <c r="H29" s="25" t="n"/>
+      <c r="I29" s="25" t="n"/>
+      <c r="J29" s="25" t="n"/>
+      <c r="K29" s="27" t="n"/>
+      <c r="L29" s="27" t="n"/>
+      <c r="M29" s="27" t="n"/>
+      <c r="N29" s="27" t="n"/>
+      <c r="O29" s="27" t="n"/>
+      <c r="P29" s="27" t="n"/>
+      <c r="Q29" s="27" t="n"/>
+      <c r="R29" s="27" t="n"/>
+      <c r="S29" s="58" t="n"/>
+      <c r="T29" s="27" t="n"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="25" t="n">
+        <v>20</v>
+      </c>
+      <c r="B30" s="25" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="C30" s="25" t="n"/>
+      <c r="D30" s="25" t="n"/>
+      <c r="E30" s="25" t="n"/>
+      <c r="F30" s="25" t="n"/>
+      <c r="G30" s="25" t="n"/>
+      <c r="H30" s="25" t="n"/>
+      <c r="I30" s="25" t="n"/>
+      <c r="J30" s="25" t="n"/>
+      <c r="K30" s="27" t="n"/>
+      <c r="L30" s="27" t="n"/>
+      <c r="M30" s="27" t="n"/>
+      <c r="N30" s="27" t="n"/>
+      <c r="O30" s="27" t="n"/>
+      <c r="P30" s="27" t="n"/>
+      <c r="Q30" s="27" t="n"/>
+      <c r="R30" s="27" t="n"/>
+      <c r="S30" s="58" t="n"/>
+      <c r="T30" s="27" t="n"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="25" t="n">
+        <v>21</v>
+      </c>
+      <c r="B31" s="25" t="inlineStr">
+        <is>
+          <t>Sáb</t>
+        </is>
+      </c>
+      <c r="C31" s="60" t="n"/>
+      <c r="D31" s="60" t="n"/>
+      <c r="E31" s="60" t="n"/>
+      <c r="F31" s="60" t="n"/>
+      <c r="G31" s="60" t="n"/>
+      <c r="H31" s="60" t="n"/>
+      <c r="I31" s="60" t="n"/>
+      <c r="J31" s="60" t="n"/>
+      <c r="K31" s="61" t="n"/>
+      <c r="L31" s="61" t="n"/>
+      <c r="M31" s="61" t="n"/>
+      <c r="N31" s="61" t="n"/>
+      <c r="O31" s="61" t="n"/>
+      <c r="P31" s="61" t="n"/>
+      <c r="Q31" s="61" t="n"/>
+      <c r="R31" s="61" t="n"/>
+      <c r="S31" s="62" t="n"/>
+      <c r="T31" s="61" t="n"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="25" t="n">
+        <v>22</v>
+      </c>
+      <c r="B32" s="25" t="inlineStr">
+        <is>
+          <t>Dom</t>
+        </is>
+      </c>
+      <c r="C32" s="60" t="n"/>
+      <c r="D32" s="60" t="n"/>
+      <c r="E32" s="60" t="n"/>
+      <c r="F32" s="60" t="n"/>
+      <c r="G32" s="60" t="n"/>
+      <c r="H32" s="60" t="n"/>
+      <c r="I32" s="60" t="n"/>
+      <c r="J32" s="60" t="n"/>
+      <c r="K32" s="61" t="n"/>
+      <c r="L32" s="61" t="n"/>
+      <c r="M32" s="61" t="n"/>
+      <c r="N32" s="61" t="n"/>
+      <c r="O32" s="61" t="n"/>
+      <c r="P32" s="61" t="n"/>
+      <c r="Q32" s="61" t="n"/>
+      <c r="R32" s="61" t="n"/>
+      <c r="S32" s="62" t="n"/>
+      <c r="T32" s="61" t="n"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="25" t="n">
+        <v>23</v>
+      </c>
+      <c r="B33" s="25" t="inlineStr">
+        <is>
+          <t>Seg</t>
+        </is>
+      </c>
+      <c r="C33" s="25" t="n"/>
+      <c r="D33" s="25" t="n"/>
+      <c r="E33" s="25" t="n"/>
+      <c r="F33" s="25" t="n"/>
+      <c r="G33" s="25" t="n"/>
+      <c r="H33" s="25" t="n"/>
+      <c r="I33" s="25" t="n"/>
+      <c r="J33" s="25" t="n"/>
+      <c r="K33" s="27" t="n"/>
+      <c r="L33" s="27" t="n"/>
+      <c r="M33" s="27" t="n"/>
+      <c r="N33" s="27" t="n"/>
+      <c r="O33" s="27" t="n"/>
+      <c r="P33" s="27" t="n"/>
+      <c r="Q33" s="27" t="n"/>
+      <c r="R33" s="27" t="n"/>
+      <c r="S33" s="58" t="n"/>
+      <c r="T33" s="27" t="n"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B34" s="25" t="inlineStr">
+        <is>
+          <t>Ter</t>
+        </is>
+      </c>
+      <c r="C34" s="25" t="n"/>
+      <c r="D34" s="25" t="n"/>
+      <c r="E34" s="25" t="n"/>
+      <c r="F34" s="25" t="n"/>
+      <c r="G34" s="25" t="n"/>
+      <c r="H34" s="25" t="n"/>
+      <c r="I34" s="25" t="n"/>
+      <c r="J34" s="25" t="n"/>
+      <c r="K34" s="27" t="n"/>
+      <c r="L34" s="27" t="n"/>
+      <c r="M34" s="27" t="n"/>
+      <c r="N34" s="27" t="n"/>
+      <c r="O34" s="27" t="n"/>
+      <c r="P34" s="27" t="n"/>
+      <c r="Q34" s="27" t="n"/>
+      <c r="R34" s="27" t="n"/>
+      <c r="S34" s="58" t="n"/>
+      <c r="T34" s="27" t="n"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="25" t="n">
+        <v>25</v>
+      </c>
+      <c r="B35" s="25" t="inlineStr">
+        <is>
+          <t>Qua</t>
+        </is>
+      </c>
+      <c r="C35" s="25" t="n"/>
+      <c r="D35" s="25" t="n"/>
+      <c r="E35" s="25" t="n"/>
+      <c r="F35" s="25" t="n"/>
+      <c r="G35" s="25" t="n"/>
+      <c r="H35" s="25" t="n"/>
+      <c r="I35" s="25" t="n"/>
+      <c r="J35" s="25" t="n"/>
+      <c r="K35" s="27" t="n"/>
+      <c r="L35" s="27" t="n"/>
+      <c r="M35" s="27" t="n"/>
+      <c r="N35" s="27" t="n"/>
+      <c r="O35" s="27" t="n"/>
+      <c r="P35" s="27" t="n"/>
+      <c r="Q35" s="27" t="n"/>
+      <c r="R35" s="27" t="n"/>
+      <c r="S35" s="58" t="n"/>
+      <c r="T35" s="27" t="n"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="25" t="n">
+        <v>26</v>
+      </c>
+      <c r="B36" s="25" t="inlineStr">
+        <is>
+          <t>Qui</t>
+        </is>
+      </c>
+      <c r="C36" s="25" t="n"/>
+      <c r="D36" s="25" t="n"/>
+      <c r="E36" s="25" t="n"/>
+      <c r="F36" s="25" t="n"/>
+      <c r="G36" s="25" t="n"/>
+      <c r="H36" s="25" t="n"/>
+      <c r="I36" s="25" t="n"/>
+      <c r="J36" s="25" t="n"/>
+      <c r="K36" s="27" t="n"/>
+      <c r="L36" s="27" t="n"/>
+      <c r="M36" s="27" t="n"/>
+      <c r="N36" s="27" t="n"/>
+      <c r="O36" s="27" t="n"/>
+      <c r="P36" s="27" t="n"/>
+      <c r="Q36" s="27" t="n"/>
+      <c r="R36" s="27" t="n"/>
+      <c r="S36" s="58" t="n"/>
+      <c r="T36" s="27" t="n"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="25" t="n">
+        <v>27</v>
+      </c>
+      <c r="B37" s="25" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="C37" s="25" t="n"/>
+      <c r="D37" s="25" t="n"/>
+      <c r="E37" s="25" t="n"/>
+      <c r="F37" s="25" t="n"/>
+      <c r="G37" s="25" t="n"/>
+      <c r="H37" s="25" t="n"/>
+      <c r="I37" s="25" t="n"/>
+      <c r="J37" s="25" t="n"/>
+      <c r="K37" s="27" t="n"/>
+      <c r="L37" s="27" t="n"/>
+      <c r="M37" s="27" t="n"/>
+      <c r="N37" s="27" t="n"/>
+      <c r="O37" s="27" t="n"/>
+      <c r="P37" s="27" t="n"/>
+      <c r="Q37" s="27" t="n"/>
+      <c r="R37" s="27" t="n"/>
+      <c r="S37" s="58" t="n"/>
+      <c r="T37" s="27" t="n"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="25" t="n">
+        <v>28</v>
+      </c>
+      <c r="B38" s="25" t="inlineStr">
+        <is>
+          <t>Sáb</t>
+        </is>
+      </c>
+      <c r="C38" s="60" t="n"/>
+      <c r="D38" s="60" t="n"/>
+      <c r="E38" s="60" t="n"/>
+      <c r="F38" s="60" t="n"/>
+      <c r="G38" s="60" t="n"/>
+      <c r="H38" s="60" t="n"/>
+      <c r="I38" s="60" t="n"/>
+      <c r="J38" s="60" t="n"/>
+      <c r="K38" s="61" t="n"/>
+      <c r="L38" s="61" t="n"/>
+      <c r="M38" s="61" t="n"/>
+      <c r="N38" s="61" t="n"/>
+      <c r="O38" s="61" t="n"/>
+      <c r="P38" s="61" t="n"/>
+      <c r="Q38" s="61" t="n"/>
+      <c r="R38" s="61" t="n"/>
+      <c r="S38" s="62" t="n"/>
+      <c r="T38" s="61" t="n"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="25" t="n">
+        <v>29</v>
+      </c>
+      <c r="B39" s="25" t="inlineStr">
+        <is>
+          <t>Dom</t>
+        </is>
+      </c>
+      <c r="C39" s="60" t="n"/>
+      <c r="D39" s="60" t="n"/>
+      <c r="E39" s="60" t="n"/>
+      <c r="F39" s="60" t="n"/>
+      <c r="G39" s="60" t="n"/>
+      <c r="H39" s="60" t="n"/>
+      <c r="I39" s="60" t="n"/>
+      <c r="J39" s="60" t="n"/>
+      <c r="K39" s="61" t="n"/>
+      <c r="L39" s="61" t="n"/>
+      <c r="M39" s="61" t="n"/>
+      <c r="N39" s="61" t="n"/>
+      <c r="O39" s="61" t="n"/>
+      <c r="P39" s="61" t="n"/>
+      <c r="Q39" s="61" t="n"/>
+      <c r="R39" s="61" t="n"/>
+      <c r="S39" s="62" t="n"/>
+      <c r="T39" s="61" t="n"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="25" t="n">
+        <v>30</v>
+      </c>
+      <c r="B40" s="25" t="inlineStr">
+        <is>
+          <t>Seg</t>
+        </is>
+      </c>
+      <c r="C40" s="25" t="n"/>
+      <c r="D40" s="25" t="n"/>
+      <c r="E40" s="25" t="n"/>
+      <c r="F40" s="25" t="n"/>
+      <c r="G40" s="25" t="n"/>
+      <c r="H40" s="25" t="n"/>
+      <c r="I40" s="25" t="n"/>
+      <c r="J40" s="25" t="n"/>
+      <c r="K40" s="27" t="n"/>
+      <c r="L40" s="27" t="n"/>
+      <c r="M40" s="27" t="n"/>
+      <c r="N40" s="27" t="n"/>
+      <c r="O40" s="27" t="n"/>
+      <c r="P40" s="27" t="n"/>
+      <c r="Q40" s="27" t="n"/>
+      <c r="R40" s="27" t="n"/>
+      <c r="S40" s="58" t="n"/>
+      <c r="T40" s="27" t="n"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="25" t="n">
+        <v>31</v>
+      </c>
+      <c r="B41" s="25" t="inlineStr">
+        <is>
+          <t>Ter</t>
+        </is>
+      </c>
+      <c r="C41" s="25" t="n"/>
+      <c r="D41" s="25" t="n"/>
+      <c r="E41" s="25" t="n"/>
+      <c r="F41" s="25" t="n"/>
+      <c r="G41" s="25" t="n"/>
+      <c r="H41" s="25" t="n"/>
+      <c r="I41" s="25" t="n"/>
+      <c r="J41" s="25" t="n"/>
+      <c r="K41" s="27" t="n"/>
+      <c r="L41" s="27" t="n"/>
+      <c r="M41" s="27" t="n"/>
+      <c r="N41" s="27" t="n"/>
+      <c r="O41" s="27" t="n"/>
+      <c r="P41" s="27" t="n"/>
+      <c r="Q41" s="27" t="n"/>
+      <c r="R41" s="27" t="n"/>
+      <c r="S41" s="58" t="n"/>
+      <c r="T41" s="27" t="n"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="25" t="n"/>
+      <c r="B42" s="25" t="n"/>
+      <c r="C42" s="25" t="n"/>
+      <c r="D42" s="25" t="n"/>
+      <c r="E42" s="25" t="n"/>
+      <c r="F42" s="25" t="n"/>
+      <c r="G42" s="25" t="n"/>
+      <c r="H42" s="25" t="n"/>
+      <c r="I42" s="25" t="n"/>
+      <c r="J42" s="25" t="n"/>
+      <c r="K42" s="27" t="n"/>
+      <c r="L42" s="27" t="n"/>
+      <c r="M42" s="27" t="n"/>
+      <c r="N42" s="27" t="n"/>
+      <c r="O42" s="27" t="n"/>
+      <c r="P42" s="27" t="n"/>
+      <c r="Q42" s="27" t="n"/>
+      <c r="R42" s="27" t="n"/>
+      <c r="S42" s="58" t="n"/>
+      <c r="T42" s="27" t="n"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="25" t="n"/>
+      <c r="B43" s="25" t="n"/>
+      <c r="C43" s="25" t="n"/>
+      <c r="D43" s="25" t="n"/>
+      <c r="E43" s="25" t="n"/>
+      <c r="F43" s="25" t="n"/>
+      <c r="G43" s="25" t="n"/>
+      <c r="H43" s="25" t="n"/>
+      <c r="I43" s="25" t="n"/>
+      <c r="J43" s="25" t="n"/>
+      <c r="K43" s="27" t="n"/>
+      <c r="L43" s="27" t="n"/>
+      <c r="M43" s="27" t="n"/>
+      <c r="N43" s="27" t="n"/>
+      <c r="O43" s="27" t="n"/>
+      <c r="P43" s="27" t="n"/>
+      <c r="Q43" s="27" t="n"/>
+      <c r="R43" s="27" t="n"/>
+      <c r="S43" s="58" t="n"/>
+      <c r="T43" s="27" t="n"/>
+    </row>
+    <row r="44" ht="15.75" customHeight="1" s="20" thickBot="1"/>
+    <row r="45">
+      <c r="A45" s="16" t="n"/>
+      <c r="B45" s="17" t="n"/>
+      <c r="C45" s="17" t="n"/>
+      <c r="D45" s="17" t="n"/>
+      <c r="E45" s="17" t="n"/>
+      <c r="F45" s="17" t="n"/>
+      <c r="G45" s="17" t="n"/>
+      <c r="H45" s="17" t="n"/>
+      <c r="I45" s="17" t="n"/>
+      <c r="J45" s="18" t="n"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="19" t="n"/>
+      <c r="J46" s="21" t="n"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="19" t="n"/>
+      <c r="J47" s="21" t="n"/>
+    </row>
+    <row r="48" ht="15.75" customHeight="1" s="20" thickBot="1">
+      <c r="A48" s="22" t="n"/>
+      <c r="B48" s="23" t="n"/>
+      <c r="C48" s="23" t="n"/>
+      <c r="D48" s="23" t="n"/>
+      <c r="E48" s="23" t="n"/>
+      <c r="F48" s="23" t="n"/>
+      <c r="G48" s="23" t="n"/>
+      <c r="H48" s="23" t="n"/>
+      <c r="I48" s="23" t="n"/>
+      <c r="J48" s="24" t="n"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="I8:R8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:T9"/>
+    <mergeCell ref="L6:R6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="L7:R7"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H6:K6"/>
+  </mergeCells>
+  <pageMargins left="0.3937007874015748" right="0.3937007874015748" top="0.3937007874015748" bottom="0.3937007874015748" header="0" footer="0"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:T48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="3" bestFit="1" customWidth="1" style="20" min="1" max="1"/>
+    <col width="5.42578125" bestFit="1" customWidth="1" style="20" min="2" max="2"/>
+    <col width="26.7109375" customWidth="1" style="20" min="3" max="3"/>
+    <col width="2.7109375" customWidth="1" style="20" min="4" max="18"/>
+    <col width="13.7109375" customWidth="1" style="20" min="19" max="19"/>
+    <col width="6.28515625" customWidth="1" style="20" min="20" max="20"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="16" t="n"/>
+      <c r="B1" s="17" t="n"/>
+      <c r="C1" s="17" t="n"/>
+      <c r="D1" s="17" t="n"/>
+      <c r="E1" s="17" t="n"/>
+      <c r="F1" s="17" t="n"/>
+      <c r="G1" s="17" t="n"/>
+      <c r="H1" s="17" t="n"/>
+      <c r="I1" s="17" t="n"/>
+      <c r="J1" s="17" t="n"/>
+      <c r="K1" s="17" t="n"/>
+      <c r="L1" s="17" t="n"/>
+      <c r="M1" s="17" t="n"/>
+      <c r="N1" s="17" t="n"/>
+      <c r="O1" s="17" t="n"/>
+      <c r="P1" s="17" t="n"/>
+      <c r="Q1" s="17" t="n"/>
+      <c r="R1" s="17" t="n"/>
+      <c r="S1" s="17" t="n"/>
+      <c r="T1" s="18" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="19" t="n"/>
+      <c r="T2" s="21" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="19" t="n"/>
+      <c r="T3" s="21" t="n"/>
+    </row>
+    <row r="4" ht="15.75" customHeight="1" s="20" thickBot="1">
+      <c r="A4" s="22" t="n"/>
+      <c r="B4" s="23" t="n"/>
+      <c r="C4" s="23" t="n"/>
+      <c r="D4" s="23" t="n"/>
+      <c r="E4" s="23" t="n"/>
+      <c r="F4" s="23" t="n"/>
+      <c r="G4" s="23" t="n"/>
+      <c r="H4" s="23" t="n"/>
+      <c r="I4" s="23" t="n"/>
+      <c r="J4" s="23" t="n"/>
+      <c r="K4" s="23" t="n"/>
+      <c r="L4" s="23" t="n"/>
+      <c r="M4" s="23" t="n"/>
+      <c r="N4" s="23" t="n"/>
+      <c r="O4" s="23" t="n"/>
+      <c r="P4" s="23" t="n"/>
+      <c r="Q4" s="23" t="n"/>
+      <c r="R4" s="23" t="n"/>
+      <c r="S4" s="23" t="inlineStr">
+        <is>
+          <t>Março 2020</t>
+        </is>
+      </c>
+      <c r="T4" s="24" t="n"/>
+    </row>
+    <row r="5" ht="8.1" customHeight="1" s="20" thickBot="1"/>
+    <row r="6" ht="30" customHeight="1" s="20">
+      <c r="A6" s="41" t="inlineStr">
+        <is>
+          <t>NOME</t>
+        </is>
+      </c>
+      <c r="B6" s="17" t="n"/>
+      <c r="C6" s="30" t="inlineStr">
+        <is>
+          <t>ALIDIO GONÇALVES</t>
+        </is>
+      </c>
+      <c r="D6" s="42" t="inlineStr">
+        <is>
+          <t>RF/Vinculo</t>
+        </is>
+      </c>
+      <c r="E6" s="17" t="n"/>
+      <c r="F6" s="17" t="n"/>
+      <c r="G6" s="17" t="n"/>
+      <c r="H6" s="47" t="inlineStr">
+        <is>
+          <t>819.027.5/2</t>
+        </is>
+      </c>
+      <c r="I6" s="17" t="n"/>
+      <c r="J6" s="17" t="n"/>
+      <c r="K6" s="17" t="n"/>
+      <c r="L6" s="38" t="inlineStr">
+        <is>
+          <t>Estrutura Hierárquica</t>
+        </is>
+      </c>
+      <c r="M6" s="17" t="n"/>
+      <c r="N6" s="17" t="n"/>
+      <c r="O6" s="17" t="n"/>
+      <c r="P6" s="17" t="n"/>
+      <c r="Q6" s="17" t="n"/>
+      <c r="R6" s="17" t="n"/>
+      <c r="S6" s="59" t="inlineStr">
+        <is>
+          <t>162500000630000</t>
+        </is>
+      </c>
+      <c r="T6" s="18" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CARGO </t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Professor Educ. Infantil e Ens. Fund. I</t>
+        </is>
+      </c>
+      <c r="D7" s="44" t="inlineStr">
+        <is>
+          <t>QPE</t>
+        </is>
+      </c>
+      <c r="H7" s="45" t="inlineStr">
+        <is>
+          <t>4A</t>
+        </is>
+      </c>
+      <c r="L7" s="44" t="inlineStr">
+        <is>
+          <t>JORNADA</t>
+        </is>
+      </c>
+      <c r="S7" s="46" t="inlineStr">
+        <is>
+          <t>JBD</t>
+        </is>
+      </c>
+      <c r="T7" s="21" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="48" t="inlineStr">
+        <is>
+          <t>regência</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>11:00 - 15:00 HS</t>
+        </is>
+      </c>
+      <c r="D8" s="44" t="inlineStr">
+        <is>
+          <t>hor. Coletivo</t>
+        </is>
+      </c>
+      <c r="I8" s="45" t="inlineStr">
+        <is>
+          <t>15:00 - 16:30 HS</t>
+        </is>
+      </c>
+      <c r="S8" s="44" t="inlineStr">
+        <is>
+          <t>turma</t>
+        </is>
+      </c>
+      <c r="T8" s="46" t="inlineStr">
+        <is>
+          <t>7A</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="15.75" customHeight="1" s="20" thickBot="1">
+      <c r="A9" s="50" t="inlineStr">
+        <is>
+          <t>H.A / H.I</t>
+        </is>
+      </c>
+      <c r="B9" s="23" t="n"/>
+      <c r="C9" s="53" t="inlineStr">
+        <is>
+          <t>segunda 10:15 - 11:00; quarta 10:15 - 11:00hs</t>
+        </is>
+      </c>
+      <c r="D9" s="23" t="n"/>
+      <c r="E9" s="23" t="n"/>
+      <c r="F9" s="23" t="n"/>
+      <c r="G9" s="23" t="n"/>
+      <c r="H9" s="23" t="n"/>
+      <c r="I9" s="23" t="n"/>
+      <c r="J9" s="23" t="n"/>
+      <c r="K9" s="23" t="n"/>
+      <c r="L9" s="23" t="n"/>
+      <c r="M9" s="23" t="n"/>
+      <c r="N9" s="23" t="n"/>
+      <c r="O9" s="23" t="n"/>
+      <c r="P9" s="23" t="n"/>
+      <c r="Q9" s="23" t="n"/>
+      <c r="R9" s="23" t="n"/>
+      <c r="S9" s="23" t="n"/>
+      <c r="T9" s="24" t="n"/>
+    </row>
+    <row r="10" ht="16.5" customHeight="1" s="20"/>
+    <row r="11">
+      <c r="A11" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" s="25" t="inlineStr">
+        <is>
+          <t>Dom</t>
+        </is>
+      </c>
+      <c r="C11" s="60" t="n"/>
+      <c r="D11" s="60" t="n"/>
+      <c r="E11" s="60" t="n"/>
+      <c r="F11" s="60" t="n"/>
+      <c r="G11" s="60" t="n"/>
+      <c r="H11" s="60" t="n"/>
+      <c r="I11" s="60" t="n"/>
+      <c r="J11" s="60" t="n"/>
+      <c r="K11" s="61" t="n"/>
+      <c r="L11" s="61" t="n"/>
+      <c r="M11" s="61" t="n"/>
+      <c r="N11" s="61" t="n"/>
+      <c r="O11" s="61" t="n"/>
+      <c r="P11" s="61" t="n"/>
+      <c r="Q11" s="61" t="n"/>
+      <c r="R11" s="61" t="n"/>
+      <c r="S11" s="62" t="n"/>
+      <c r="T11" s="61" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" s="25" t="inlineStr">
+        <is>
+          <t>Seg</t>
+        </is>
+      </c>
+      <c r="C12" s="25" t="n"/>
+      <c r="D12" s="25" t="n"/>
+      <c r="E12" s="25" t="n"/>
+      <c r="F12" s="25" t="n"/>
+      <c r="G12" s="25" t="n"/>
+      <c r="H12" s="25" t="n"/>
+      <c r="I12" s="25" t="n"/>
+      <c r="J12" s="25" t="n"/>
+      <c r="K12" s="27" t="n"/>
+      <c r="L12" s="27" t="n"/>
+      <c r="M12" s="27" t="n"/>
+      <c r="N12" s="27" t="n"/>
+      <c r="O12" s="27" t="n"/>
+      <c r="P12" s="27" t="n"/>
+      <c r="Q12" s="27" t="n"/>
+      <c r="R12" s="27" t="n"/>
+      <c r="S12" s="58" t="n"/>
+      <c r="T12" s="27" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="B13" s="25" t="inlineStr">
+        <is>
+          <t>Ter</t>
+        </is>
+      </c>
+      <c r="C13" s="25" t="n"/>
+      <c r="D13" s="25" t="n"/>
+      <c r="E13" s="25" t="n"/>
+      <c r="F13" s="25" t="n"/>
+      <c r="G13" s="25" t="n"/>
+      <c r="H13" s="26" t="n"/>
+      <c r="I13" s="25" t="n"/>
+      <c r="J13" s="25" t="n"/>
+      <c r="K13" s="27" t="n"/>
+      <c r="L13" s="27" t="n"/>
+      <c r="M13" s="27" t="n"/>
+      <c r="N13" s="27" t="n"/>
+      <c r="O13" s="27" t="n"/>
+      <c r="P13" s="27" t="n"/>
+      <c r="Q13" s="27" t="n"/>
+      <c r="R13" s="27" t="n"/>
+      <c r="S13" s="58" t="n"/>
+      <c r="T13" s="27" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="B14" s="25" t="inlineStr">
+        <is>
+          <t>Qua</t>
+        </is>
+      </c>
+      <c r="C14" s="25" t="n"/>
+      <c r="D14" s="25" t="n"/>
+      <c r="E14" s="25" t="n"/>
+      <c r="F14" s="25" t="n"/>
+      <c r="G14" s="25" t="n"/>
+      <c r="H14" s="25" t="n"/>
+      <c r="I14" s="25" t="n"/>
+      <c r="J14" s="25" t="n"/>
+      <c r="K14" s="27" t="n"/>
+      <c r="L14" s="27" t="n"/>
+      <c r="M14" s="27" t="n"/>
+      <c r="N14" s="27" t="n"/>
+      <c r="O14" s="27" t="n"/>
+      <c r="P14" s="27" t="n"/>
+      <c r="Q14" s="27" t="n"/>
+      <c r="R14" s="27" t="n"/>
+      <c r="S14" s="58" t="n"/>
+      <c r="T14" s="27" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="25" t="n">
+        <v>5</v>
+      </c>
+      <c r="B15" s="25" t="inlineStr">
+        <is>
+          <t>Qui</t>
+        </is>
+      </c>
+      <c r="C15" s="25" t="n"/>
+      <c r="D15" s="25" t="n"/>
+      <c r="E15" s="25" t="n"/>
+      <c r="F15" s="25" t="n"/>
+      <c r="G15" s="25" t="n"/>
+      <c r="H15" s="25" t="n"/>
+      <c r="I15" s="25" t="n"/>
+      <c r="J15" s="25" t="n"/>
+      <c r="K15" s="27" t="n"/>
+      <c r="L15" s="27" t="n"/>
+      <c r="M15" s="27" t="n"/>
+      <c r="N15" s="27" t="n"/>
+      <c r="O15" s="27" t="n"/>
+      <c r="P15" s="27" t="n"/>
+      <c r="Q15" s="27" t="n"/>
+      <c r="R15" s="27" t="n"/>
+      <c r="S15" s="58" t="n"/>
+      <c r="T15" s="27" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="25" t="n">
+        <v>6</v>
+      </c>
+      <c r="B16" s="25" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="C16" s="25" t="n"/>
+      <c r="D16" s="25" t="n"/>
+      <c r="E16" s="25" t="n"/>
+      <c r="F16" s="25" t="n"/>
+      <c r="G16" s="25" t="n"/>
+      <c r="H16" s="25" t="n"/>
+      <c r="I16" s="25" t="n"/>
+      <c r="J16" s="25" t="n"/>
+      <c r="K16" s="27" t="n"/>
+      <c r="L16" s="27" t="n"/>
+      <c r="M16" s="27" t="n"/>
+      <c r="N16" s="27" t="n"/>
+      <c r="O16" s="27" t="n"/>
+      <c r="P16" s="27" t="n"/>
+      <c r="Q16" s="27" t="n"/>
+      <c r="R16" s="27" t="n"/>
+      <c r="S16" s="58" t="n"/>
+      <c r="T16" s="27" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="B17" s="25" t="inlineStr">
+        <is>
+          <t>Sáb</t>
+        </is>
+      </c>
+      <c r="C17" s="60" t="n"/>
+      <c r="D17" s="60" t="n"/>
+      <c r="E17" s="60" t="n"/>
+      <c r="F17" s="60" t="n"/>
+      <c r="G17" s="60" t="n"/>
+      <c r="H17" s="60" t="n"/>
+      <c r="I17" s="60" t="n"/>
+      <c r="J17" s="60" t="n"/>
+      <c r="K17" s="61" t="n"/>
+      <c r="L17" s="61" t="n"/>
+      <c r="M17" s="61" t="n"/>
+      <c r="N17" s="61" t="n"/>
+      <c r="O17" s="61" t="n"/>
+      <c r="P17" s="61" t="n"/>
+      <c r="Q17" s="61" t="n"/>
+      <c r="R17" s="61" t="n"/>
+      <c r="S17" s="62" t="n"/>
+      <c r="T17" s="61" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="B18" s="25" t="inlineStr">
+        <is>
+          <t>Dom</t>
+        </is>
+      </c>
+      <c r="C18" s="60" t="n"/>
+      <c r="D18" s="60" t="n"/>
+      <c r="E18" s="60" t="n"/>
+      <c r="F18" s="60" t="n"/>
+      <c r="G18" s="60" t="n"/>
+      <c r="H18" s="60" t="n"/>
+      <c r="I18" s="60" t="n"/>
+      <c r="J18" s="60" t="n"/>
+      <c r="K18" s="61" t="n"/>
+      <c r="L18" s="61" t="n"/>
+      <c r="M18" s="61" t="n"/>
+      <c r="N18" s="61" t="n"/>
+      <c r="O18" s="61" t="n"/>
+      <c r="P18" s="61" t="n"/>
+      <c r="Q18" s="61" t="n"/>
+      <c r="R18" s="61" t="n"/>
+      <c r="S18" s="62" t="n"/>
+      <c r="T18" s="61" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="25" t="n">
+        <v>9</v>
+      </c>
+      <c r="B19" s="25" t="inlineStr">
+        <is>
+          <t>Seg</t>
+        </is>
+      </c>
+      <c r="C19" s="25" t="n"/>
+      <c r="D19" s="25" t="n"/>
+      <c r="E19" s="25" t="n"/>
+      <c r="F19" s="25" t="n"/>
+      <c r="G19" s="25" t="n"/>
+      <c r="H19" s="25" t="n"/>
+      <c r="I19" s="25" t="n"/>
+      <c r="J19" s="25" t="n"/>
+      <c r="K19" s="27" t="n"/>
+      <c r="L19" s="27" t="n"/>
+      <c r="M19" s="27" t="n"/>
+      <c r="N19" s="27" t="n"/>
+      <c r="O19" s="27" t="n"/>
+      <c r="P19" s="27" t="n"/>
+      <c r="Q19" s="27" t="n"/>
+      <c r="R19" s="27" t="n"/>
+      <c r="S19" s="58" t="n"/>
+      <c r="T19" s="27" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="25" t="n">
+        <v>10</v>
+      </c>
+      <c r="B20" s="25" t="inlineStr">
+        <is>
+          <t>Ter</t>
+        </is>
+      </c>
+      <c r="C20" s="25" t="n"/>
+      <c r="D20" s="25" t="n"/>
+      <c r="E20" s="25" t="n"/>
+      <c r="F20" s="25" t="n"/>
+      <c r="G20" s="25" t="n"/>
+      <c r="H20" s="25" t="n"/>
+      <c r="I20" s="25" t="n"/>
+      <c r="J20" s="25" t="n"/>
+      <c r="K20" s="27" t="n"/>
+      <c r="L20" s="27" t="n"/>
+      <c r="M20" s="27" t="n"/>
+      <c r="N20" s="27" t="n"/>
+      <c r="O20" s="27" t="n"/>
+      <c r="P20" s="27" t="n"/>
+      <c r="Q20" s="27" t="n"/>
+      <c r="R20" s="27" t="n"/>
+      <c r="S20" s="58" t="n"/>
+      <c r="T20" s="27" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="25" t="n">
+        <v>11</v>
+      </c>
+      <c r="B21" s="25" t="inlineStr">
+        <is>
+          <t>Qua</t>
+        </is>
+      </c>
+      <c r="C21" s="25" t="n"/>
+      <c r="D21" s="25" t="n"/>
+      <c r="E21" s="25" t="n"/>
+      <c r="F21" s="25" t="n"/>
+      <c r="G21" s="25" t="n"/>
+      <c r="H21" s="25" t="n"/>
+      <c r="I21" s="25" t="n"/>
+      <c r="J21" s="25" t="n"/>
+      <c r="K21" s="27" t="n"/>
+      <c r="L21" s="27" t="n"/>
+      <c r="M21" s="27" t="n"/>
+      <c r="N21" s="27" t="n"/>
+      <c r="O21" s="27" t="n"/>
+      <c r="P21" s="27" t="n"/>
+      <c r="Q21" s="27" t="n"/>
+      <c r="R21" s="27" t="n"/>
+      <c r="S21" s="58" t="n"/>
+      <c r="T21" s="27" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="25" t="n">
+        <v>12</v>
+      </c>
+      <c r="B22" s="25" t="inlineStr">
+        <is>
+          <t>Qui</t>
+        </is>
+      </c>
+      <c r="C22" s="25" t="n"/>
+      <c r="D22" s="25" t="n"/>
+      <c r="E22" s="25" t="n"/>
+      <c r="F22" s="25" t="n"/>
+      <c r="G22" s="25" t="n"/>
+      <c r="H22" s="25" t="n"/>
+      <c r="I22" s="25" t="n"/>
+      <c r="J22" s="25" t="n"/>
+      <c r="K22" s="27" t="n"/>
+      <c r="L22" s="27" t="n"/>
+      <c r="M22" s="27" t="n"/>
+      <c r="N22" s="27" t="n"/>
+      <c r="O22" s="27" t="n"/>
+      <c r="P22" s="27" t="n"/>
+      <c r="Q22" s="27" t="n"/>
+      <c r="R22" s="27" t="n"/>
+      <c r="S22" s="58" t="n"/>
+      <c r="T22" s="27" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="25" t="n">
+        <v>13</v>
+      </c>
+      <c r="B23" s="25" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="C23" s="25" t="n"/>
+      <c r="D23" s="25" t="n"/>
+      <c r="E23" s="25" t="n"/>
+      <c r="F23" s="25" t="n"/>
+      <c r="G23" s="25" t="n"/>
+      <c r="H23" s="25" t="n"/>
+      <c r="I23" s="25" t="n"/>
+      <c r="J23" s="25" t="n"/>
+      <c r="K23" s="27" t="n"/>
+      <c r="L23" s="27" t="n"/>
+      <c r="M23" s="27" t="n"/>
+      <c r="N23" s="27" t="n"/>
+      <c r="O23" s="27" t="n"/>
+      <c r="P23" s="27" t="n"/>
+      <c r="Q23" s="27" t="n"/>
+      <c r="R23" s="27" t="n"/>
+      <c r="S23" s="58" t="n"/>
+      <c r="T23" s="27" t="n"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="25" t="n">
+        <v>14</v>
+      </c>
+      <c r="B24" s="25" t="inlineStr">
+        <is>
+          <t>Sáb</t>
+        </is>
+      </c>
+      <c r="C24" s="60" t="n"/>
+      <c r="D24" s="60" t="n"/>
+      <c r="E24" s="60" t="n"/>
+      <c r="F24" s="60" t="n"/>
+      <c r="G24" s="60" t="n"/>
+      <c r="H24" s="60" t="n"/>
+      <c r="I24" s="60" t="n"/>
+      <c r="J24" s="60" t="n"/>
+      <c r="K24" s="61" t="n"/>
+      <c r="L24" s="61" t="n"/>
+      <c r="M24" s="61" t="n"/>
+      <c r="N24" s="61" t="n"/>
+      <c r="O24" s="61" t="n"/>
+      <c r="P24" s="61" t="n"/>
+      <c r="Q24" s="61" t="n"/>
+      <c r="R24" s="61" t="n"/>
+      <c r="S24" s="62" t="n"/>
+      <c r="T24" s="61" t="n"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="25" t="n">
+        <v>15</v>
+      </c>
+      <c r="B25" s="25" t="inlineStr">
+        <is>
+          <t>Dom</t>
+        </is>
+      </c>
+      <c r="C25" s="60" t="n"/>
+      <c r="D25" s="60" t="n"/>
+      <c r="E25" s="60" t="n"/>
+      <c r="F25" s="60" t="n"/>
+      <c r="G25" s="60" t="n"/>
+      <c r="H25" s="60" t="n"/>
+      <c r="I25" s="60" t="n"/>
+      <c r="J25" s="60" t="n"/>
+      <c r="K25" s="61" t="n"/>
+      <c r="L25" s="61" t="n"/>
+      <c r="M25" s="61" t="n"/>
+      <c r="N25" s="61" t="n"/>
+      <c r="O25" s="61" t="n"/>
+      <c r="P25" s="61" t="n"/>
+      <c r="Q25" s="61" t="n"/>
+      <c r="R25" s="61" t="n"/>
+      <c r="S25" s="62" t="n"/>
+      <c r="T25" s="61" t="n"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="25" t="n">
+        <v>16</v>
+      </c>
+      <c r="B26" s="25" t="inlineStr">
+        <is>
+          <t>Seg</t>
+        </is>
+      </c>
+      <c r="C26" s="25" t="n"/>
+      <c r="D26" s="25" t="n"/>
+      <c r="E26" s="25" t="n"/>
+      <c r="F26" s="25" t="n"/>
+      <c r="G26" s="25" t="n"/>
+      <c r="H26" s="25" t="n"/>
+      <c r="I26" s="25" t="n"/>
+      <c r="J26" s="25" t="n"/>
+      <c r="K26" s="27" t="n"/>
+      <c r="L26" s="27" t="n"/>
+      <c r="M26" s="27" t="n"/>
+      <c r="N26" s="27" t="n"/>
+      <c r="O26" s="27" t="n"/>
+      <c r="P26" s="27" t="n"/>
+      <c r="Q26" s="27" t="n"/>
+      <c r="R26" s="27" t="n"/>
+      <c r="S26" s="58" t="n"/>
+      <c r="T26" s="27" t="n"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="25" t="n">
+        <v>17</v>
+      </c>
+      <c r="B27" s="25" t="inlineStr">
+        <is>
+          <t>Ter</t>
+        </is>
+      </c>
+      <c r="C27" s="25" t="n"/>
+      <c r="D27" s="25" t="n"/>
+      <c r="E27" s="25" t="n"/>
+      <c r="F27" s="25" t="n"/>
+      <c r="G27" s="25" t="n"/>
+      <c r="H27" s="25" t="n"/>
+      <c r="I27" s="25" t="n"/>
+      <c r="J27" s="25" t="n"/>
+      <c r="K27" s="27" t="n"/>
+      <c r="L27" s="27" t="n"/>
+      <c r="M27" s="27" t="n"/>
+      <c r="N27" s="27" t="n"/>
+      <c r="O27" s="27" t="n"/>
+      <c r="P27" s="27" t="n"/>
+      <c r="Q27" s="27" t="n"/>
+      <c r="R27" s="27" t="n"/>
+      <c r="S27" s="58" t="n"/>
+      <c r="T27" s="27" t="n"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="25" t="n">
+        <v>18</v>
+      </c>
+      <c r="B28" s="25" t="inlineStr">
+        <is>
+          <t>Qua</t>
+        </is>
+      </c>
+      <c r="C28" s="25" t="n"/>
+      <c r="D28" s="25" t="n"/>
+      <c r="E28" s="25" t="n"/>
+      <c r="F28" s="25" t="n"/>
+      <c r="G28" s="25" t="n"/>
+      <c r="H28" s="25" t="n"/>
+      <c r="I28" s="25" t="n"/>
+      <c r="J28" s="25" t="n"/>
+      <c r="K28" s="27" t="n"/>
+      <c r="L28" s="27" t="n"/>
+      <c r="M28" s="27" t="n"/>
+      <c r="N28" s="27" t="n"/>
+      <c r="O28" s="27" t="n"/>
+      <c r="P28" s="27" t="n"/>
+      <c r="Q28" s="27" t="n"/>
+      <c r="R28" s="27" t="n"/>
+      <c r="S28" s="58" t="n"/>
+      <c r="T28" s="27" t="n"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="25" t="n">
+        <v>19</v>
+      </c>
+      <c r="B29" s="25" t="inlineStr">
+        <is>
+          <t>Qui</t>
+        </is>
+      </c>
+      <c r="C29" s="25" t="n"/>
+      <c r="D29" s="25" t="n"/>
+      <c r="E29" s="25" t="n"/>
+      <c r="F29" s="25" t="n"/>
+      <c r="G29" s="25" t="n"/>
+      <c r="H29" s="25" t="n"/>
+      <c r="I29" s="25" t="n"/>
+      <c r="J29" s="25" t="n"/>
+      <c r="K29" s="27" t="n"/>
+      <c r="L29" s="27" t="n"/>
+      <c r="M29" s="27" t="n"/>
+      <c r="N29" s="27" t="n"/>
+      <c r="O29" s="27" t="n"/>
+      <c r="P29" s="27" t="n"/>
+      <c r="Q29" s="27" t="n"/>
+      <c r="R29" s="27" t="n"/>
+      <c r="S29" s="58" t="n"/>
+      <c r="T29" s="27" t="n"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="25" t="n">
+        <v>20</v>
+      </c>
+      <c r="B30" s="25" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="C30" s="25" t="n"/>
+      <c r="D30" s="25" t="n"/>
+      <c r="E30" s="25" t="n"/>
+      <c r="F30" s="25" t="n"/>
+      <c r="G30" s="25" t="n"/>
+      <c r="H30" s="25" t="n"/>
+      <c r="I30" s="25" t="n"/>
+      <c r="J30" s="25" t="n"/>
+      <c r="K30" s="27" t="n"/>
+      <c r="L30" s="27" t="n"/>
+      <c r="M30" s="27" t="n"/>
+      <c r="N30" s="27" t="n"/>
+      <c r="O30" s="27" t="n"/>
+      <c r="P30" s="27" t="n"/>
+      <c r="Q30" s="27" t="n"/>
+      <c r="R30" s="27" t="n"/>
+      <c r="S30" s="58" t="n"/>
+      <c r="T30" s="27" t="n"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="25" t="n">
+        <v>21</v>
+      </c>
+      <c r="B31" s="25" t="inlineStr">
+        <is>
+          <t>Sáb</t>
+        </is>
+      </c>
+      <c r="C31" s="60" t="n"/>
+      <c r="D31" s="60" t="n"/>
+      <c r="E31" s="60" t="n"/>
+      <c r="F31" s="60" t="n"/>
+      <c r="G31" s="60" t="n"/>
+      <c r="H31" s="60" t="n"/>
+      <c r="I31" s="60" t="n"/>
+      <c r="J31" s="60" t="n"/>
+      <c r="K31" s="61" t="n"/>
+      <c r="L31" s="61" t="n"/>
+      <c r="M31" s="61" t="n"/>
+      <c r="N31" s="61" t="n"/>
+      <c r="O31" s="61" t="n"/>
+      <c r="P31" s="61" t="n"/>
+      <c r="Q31" s="61" t="n"/>
+      <c r="R31" s="61" t="n"/>
+      <c r="S31" s="62" t="n"/>
+      <c r="T31" s="61" t="n"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="25" t="n">
+        <v>22</v>
+      </c>
+      <c r="B32" s="25" t="inlineStr">
+        <is>
+          <t>Dom</t>
+        </is>
+      </c>
+      <c r="C32" s="60" t="n"/>
+      <c r="D32" s="60" t="n"/>
+      <c r="E32" s="60" t="n"/>
+      <c r="F32" s="60" t="n"/>
+      <c r="G32" s="60" t="n"/>
+      <c r="H32" s="60" t="n"/>
+      <c r="I32" s="60" t="n"/>
+      <c r="J32" s="60" t="n"/>
+      <c r="K32" s="61" t="n"/>
+      <c r="L32" s="61" t="n"/>
+      <c r="M32" s="61" t="n"/>
+      <c r="N32" s="61" t="n"/>
+      <c r="O32" s="61" t="n"/>
+      <c r="P32" s="61" t="n"/>
+      <c r="Q32" s="61" t="n"/>
+      <c r="R32" s="61" t="n"/>
+      <c r="S32" s="62" t="n"/>
+      <c r="T32" s="61" t="n"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="25" t="n">
+        <v>23</v>
+      </c>
+      <c r="B33" s="25" t="inlineStr">
+        <is>
+          <t>Seg</t>
+        </is>
+      </c>
+      <c r="C33" s="25" t="n"/>
+      <c r="D33" s="25" t="n"/>
+      <c r="E33" s="25" t="n"/>
+      <c r="F33" s="25" t="n"/>
+      <c r="G33" s="25" t="n"/>
+      <c r="H33" s="25" t="n"/>
+      <c r="I33" s="25" t="n"/>
+      <c r="J33" s="25" t="n"/>
+      <c r="K33" s="27" t="n"/>
+      <c r="L33" s="27" t="n"/>
+      <c r="M33" s="27" t="n"/>
+      <c r="N33" s="27" t="n"/>
+      <c r="O33" s="27" t="n"/>
+      <c r="P33" s="27" t="n"/>
+      <c r="Q33" s="27" t="n"/>
+      <c r="R33" s="27" t="n"/>
+      <c r="S33" s="58" t="n"/>
+      <c r="T33" s="27" t="n"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B34" s="25" t="inlineStr">
+        <is>
+          <t>Ter</t>
+        </is>
+      </c>
+      <c r="C34" s="25" t="n"/>
+      <c r="D34" s="25" t="n"/>
+      <c r="E34" s="25" t="n"/>
+      <c r="F34" s="25" t="n"/>
+      <c r="G34" s="25" t="n"/>
+      <c r="H34" s="25" t="n"/>
+      <c r="I34" s="25" t="n"/>
+      <c r="J34" s="25" t="n"/>
+      <c r="K34" s="27" t="n"/>
+      <c r="L34" s="27" t="n"/>
+      <c r="M34" s="27" t="n"/>
+      <c r="N34" s="27" t="n"/>
+      <c r="O34" s="27" t="n"/>
+      <c r="P34" s="27" t="n"/>
+      <c r="Q34" s="27" t="n"/>
+      <c r="R34" s="27" t="n"/>
+      <c r="S34" s="58" t="n"/>
+      <c r="T34" s="27" t="n"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="25" t="n">
+        <v>25</v>
+      </c>
+      <c r="B35" s="25" t="inlineStr">
+        <is>
+          <t>Qua</t>
+        </is>
+      </c>
+      <c r="C35" s="25" t="n"/>
+      <c r="D35" s="25" t="n"/>
+      <c r="E35" s="25" t="n"/>
+      <c r="F35" s="25" t="n"/>
+      <c r="G35" s="25" t="n"/>
+      <c r="H35" s="25" t="n"/>
+      <c r="I35" s="25" t="n"/>
+      <c r="J35" s="25" t="n"/>
+      <c r="K35" s="27" t="n"/>
+      <c r="L35" s="27" t="n"/>
+      <c r="M35" s="27" t="n"/>
+      <c r="N35" s="27" t="n"/>
+      <c r="O35" s="27" t="n"/>
+      <c r="P35" s="27" t="n"/>
+      <c r="Q35" s="27" t="n"/>
+      <c r="R35" s="27" t="n"/>
+      <c r="S35" s="58" t="n"/>
+      <c r="T35" s="27" t="n"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="25" t="n">
+        <v>26</v>
+      </c>
+      <c r="B36" s="25" t="inlineStr">
+        <is>
+          <t>Qui</t>
+        </is>
+      </c>
+      <c r="C36" s="25" t="n"/>
+      <c r="D36" s="25" t="n"/>
+      <c r="E36" s="25" t="n"/>
+      <c r="F36" s="25" t="n"/>
+      <c r="G36" s="25" t="n"/>
+      <c r="H36" s="25" t="n"/>
+      <c r="I36" s="25" t="n"/>
+      <c r="J36" s="25" t="n"/>
+      <c r="K36" s="27" t="n"/>
+      <c r="L36" s="27" t="n"/>
+      <c r="M36" s="27" t="n"/>
+      <c r="N36" s="27" t="n"/>
+      <c r="O36" s="27" t="n"/>
+      <c r="P36" s="27" t="n"/>
+      <c r="Q36" s="27" t="n"/>
+      <c r="R36" s="27" t="n"/>
+      <c r="S36" s="58" t="n"/>
+      <c r="T36" s="27" t="n"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="25" t="n">
+        <v>27</v>
+      </c>
+      <c r="B37" s="25" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="C37" s="25" t="n"/>
+      <c r="D37" s="25" t="n"/>
+      <c r="E37" s="25" t="n"/>
+      <c r="F37" s="25" t="n"/>
+      <c r="G37" s="25" t="n"/>
+      <c r="H37" s="25" t="n"/>
+      <c r="I37" s="25" t="n"/>
+      <c r="J37" s="25" t="n"/>
+      <c r="K37" s="27" t="n"/>
+      <c r="L37" s="27" t="n"/>
+      <c r="M37" s="27" t="n"/>
+      <c r="N37" s="27" t="n"/>
+      <c r="O37" s="27" t="n"/>
+      <c r="P37" s="27" t="n"/>
+      <c r="Q37" s="27" t="n"/>
+      <c r="R37" s="27" t="n"/>
+      <c r="S37" s="58" t="n"/>
+      <c r="T37" s="27" t="n"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="25" t="n">
+        <v>28</v>
+      </c>
+      <c r="B38" s="25" t="inlineStr">
+        <is>
+          <t>Sáb</t>
+        </is>
+      </c>
+      <c r="C38" s="60" t="n"/>
+      <c r="D38" s="60" t="n"/>
+      <c r="E38" s="60" t="n"/>
+      <c r="F38" s="60" t="n"/>
+      <c r="G38" s="60" t="n"/>
+      <c r="H38" s="60" t="n"/>
+      <c r="I38" s="60" t="n"/>
+      <c r="J38" s="60" t="n"/>
+      <c r="K38" s="61" t="n"/>
+      <c r="L38" s="61" t="n"/>
+      <c r="M38" s="61" t="n"/>
+      <c r="N38" s="61" t="n"/>
+      <c r="O38" s="61" t="n"/>
+      <c r="P38" s="61" t="n"/>
+      <c r="Q38" s="61" t="n"/>
+      <c r="R38" s="61" t="n"/>
+      <c r="S38" s="62" t="n"/>
+      <c r="T38" s="61" t="n"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="25" t="n">
+        <v>29</v>
+      </c>
+      <c r="B39" s="25" t="inlineStr">
+        <is>
+          <t>Dom</t>
+        </is>
+      </c>
+      <c r="C39" s="60" t="n"/>
+      <c r="D39" s="60" t="n"/>
+      <c r="E39" s="60" t="n"/>
+      <c r="F39" s="60" t="n"/>
+      <c r="G39" s="60" t="n"/>
+      <c r="H39" s="60" t="n"/>
+      <c r="I39" s="60" t="n"/>
+      <c r="J39" s="60" t="n"/>
+      <c r="K39" s="61" t="n"/>
+      <c r="L39" s="61" t="n"/>
+      <c r="M39" s="61" t="n"/>
+      <c r="N39" s="61" t="n"/>
+      <c r="O39" s="61" t="n"/>
+      <c r="P39" s="61" t="n"/>
+      <c r="Q39" s="61" t="n"/>
+      <c r="R39" s="61" t="n"/>
+      <c r="S39" s="62" t="n"/>
+      <c r="T39" s="61" t="n"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="25" t="n">
+        <v>30</v>
+      </c>
+      <c r="B40" s="25" t="inlineStr">
+        <is>
+          <t>Seg</t>
+        </is>
+      </c>
+      <c r="C40" s="25" t="n"/>
+      <c r="D40" s="25" t="n"/>
+      <c r="E40" s="25" t="n"/>
+      <c r="F40" s="25" t="n"/>
+      <c r="G40" s="25" t="n"/>
+      <c r="H40" s="25" t="n"/>
+      <c r="I40" s="25" t="n"/>
+      <c r="J40" s="25" t="n"/>
+      <c r="K40" s="27" t="n"/>
+      <c r="L40" s="27" t="n"/>
+      <c r="M40" s="27" t="n"/>
+      <c r="N40" s="27" t="n"/>
+      <c r="O40" s="27" t="n"/>
+      <c r="P40" s="27" t="n"/>
+      <c r="Q40" s="27" t="n"/>
+      <c r="R40" s="27" t="n"/>
+      <c r="S40" s="58" t="n"/>
+      <c r="T40" s="27" t="n"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="25" t="n">
+        <v>31</v>
+      </c>
+      <c r="B41" s="25" t="inlineStr">
+        <is>
+          <t>Ter</t>
+        </is>
+      </c>
+      <c r="C41" s="25" t="n"/>
+      <c r="D41" s="25" t="n"/>
+      <c r="E41" s="25" t="n"/>
+      <c r="F41" s="25" t="n"/>
+      <c r="G41" s="25" t="n"/>
+      <c r="H41" s="25" t="n"/>
+      <c r="I41" s="25" t="n"/>
+      <c r="J41" s="25" t="n"/>
+      <c r="K41" s="27" t="n"/>
+      <c r="L41" s="27" t="n"/>
+      <c r="M41" s="27" t="n"/>
+      <c r="N41" s="27" t="n"/>
+      <c r="O41" s="27" t="n"/>
+      <c r="P41" s="27" t="n"/>
+      <c r="Q41" s="27" t="n"/>
+      <c r="R41" s="27" t="n"/>
+      <c r="S41" s="58" t="n"/>
+      <c r="T41" s="27" t="n"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="25" t="n"/>
+      <c r="B42" s="25" t="n"/>
+      <c r="C42" s="25" t="n"/>
+      <c r="D42" s="25" t="n"/>
+      <c r="E42" s="25" t="n"/>
+      <c r="F42" s="25" t="n"/>
+      <c r="G42" s="25" t="n"/>
+      <c r="H42" s="25" t="n"/>
+      <c r="I42" s="25" t="n"/>
+      <c r="J42" s="25" t="n"/>
+      <c r="K42" s="27" t="n"/>
+      <c r="L42" s="27" t="n"/>
+      <c r="M42" s="27" t="n"/>
+      <c r="N42" s="27" t="n"/>
+      <c r="O42" s="27" t="n"/>
+      <c r="P42" s="27" t="n"/>
+      <c r="Q42" s="27" t="n"/>
+      <c r="R42" s="27" t="n"/>
+      <c r="S42" s="58" t="n"/>
+      <c r="T42" s="27" t="n"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="25" t="n"/>
+      <c r="B43" s="25" t="n"/>
+      <c r="C43" s="25" t="n"/>
+      <c r="D43" s="25" t="n"/>
+      <c r="E43" s="25" t="n"/>
+      <c r="F43" s="25" t="n"/>
+      <c r="G43" s="25" t="n"/>
+      <c r="H43" s="25" t="n"/>
+      <c r="I43" s="25" t="n"/>
+      <c r="J43" s="25" t="n"/>
+      <c r="K43" s="27" t="n"/>
+      <c r="L43" s="27" t="n"/>
+      <c r="M43" s="27" t="n"/>
+      <c r="N43" s="27" t="n"/>
+      <c r="O43" s="27" t="n"/>
+      <c r="P43" s="27" t="n"/>
+      <c r="Q43" s="27" t="n"/>
+      <c r="R43" s="27" t="n"/>
+      <c r="S43" s="58" t="n"/>
+      <c r="T43" s="27" t="n"/>
+    </row>
+    <row r="44" ht="15.75" customHeight="1" s="20" thickBot="1"/>
+    <row r="45">
+      <c r="A45" s="16" t="n"/>
+      <c r="B45" s="17" t="n"/>
+      <c r="C45" s="17" t="n"/>
+      <c r="D45" s="17" t="n"/>
+      <c r="E45" s="17" t="n"/>
+      <c r="F45" s="17" t="n"/>
+      <c r="G45" s="17" t="n"/>
+      <c r="H45" s="17" t="n"/>
+      <c r="I45" s="17" t="n"/>
+      <c r="J45" s="18" t="n"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="19" t="n"/>
+      <c r="J46" s="21" t="n"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="19" t="n"/>
+      <c r="J47" s="21" t="n"/>
+    </row>
+    <row r="48" ht="15.75" customHeight="1" s="20" thickBot="1">
+      <c r="A48" s="22" t="n"/>
+      <c r="B48" s="23" t="n"/>
+      <c r="C48" s="23" t="n"/>
+      <c r="D48" s="23" t="n"/>
+      <c r="E48" s="23" t="n"/>
+      <c r="F48" s="23" t="n"/>
+      <c r="G48" s="23" t="n"/>
+      <c r="H48" s="23" t="n"/>
+      <c r="I48" s="23" t="n"/>
+      <c r="J48" s="24" t="n"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="I8:R8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:T9"/>
+    <mergeCell ref="L6:R6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="L7:R7"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H6:K6"/>
+  </mergeCells>
+  <pageMargins left="0.3937007874015748" right="0.3937007874015748" top="0.3937007874015748" bottom="0.3937007874015748" header="0" footer="0"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>